<commit_message>
Updated Graphs to better show results
</commit_message>
<xml_diff>
--- a/Results Summary Laptop.xlsx
+++ b/Results Summary Laptop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\Projects\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC21F16D-A00C-400E-B3CA-7C674C19E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF82B57E-0B49-44FE-9270-927FADED8489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,27 +358,27 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>272714</xdr:colOff>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>58936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>158855</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F276FA34-872B-42FC-7A44-4B3B0D150C59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB702F8D-3ACB-A791-975C-1C339F00896F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -389,29 +389,18 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="8749964" y="1343024"/>
-          <a:ext cx="8880810" cy="5483331"/>
+          <a:off x="8620124" y="1392436"/>
+          <a:ext cx="10029825" cy="5641777"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -719,7 +708,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added NN Laptop Results
</commit_message>
<xml_diff>
--- a/Results Summary Laptop.xlsx
+++ b/Results Summary Laptop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\Projects\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF82B57E-0B49-44FE-9270-927FADED8489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB34DBE0-332C-4D8C-9C15-09A29745163C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,61 +353,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>58936</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB702F8D-3ACB-A791-975C-1C339F00896F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8620124" y="1392436"/>
-          <a:ext cx="10029825" cy="5641777"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -708,7 +653,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="B3" sqref="B3:B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,13 +735,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>423100</v>
+        <v>434200</v>
       </c>
       <c r="B3" s="14">
-        <v>2729300</v>
+        <v>2799700</v>
       </c>
       <c r="C3" s="15">
-        <v>89399500</v>
+        <v>98474800</v>
       </c>
       <c r="D3" s="13">
         <v>365000</v>
@@ -824,34 +769,34 @@
       </c>
       <c r="N3" s="1">
         <f>SUM(A$3:A$102)/100</f>
-        <v>462003</v>
+        <v>442208</v>
       </c>
       <c r="O3" s="2">
         <f>SUM(B$3:B$102)/100</f>
-        <v>2790937</v>
+        <v>2803071</v>
       </c>
       <c r="P3" s="3">
         <f>SUM(C$3:C$102)/100</f>
-        <v>91308129</v>
+        <v>97934815</v>
       </c>
       <c r="Q3" s="1">
         <f>N3/O3</f>
-        <v>0.16553687883316606</v>
+        <v>0.15775840141045303</v>
       </c>
       <c r="R3" s="3">
         <f>N3/P3</f>
-        <v>5.059823315402728E-3</v>
+        <v>4.5153299161283965E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>425900</v>
+        <v>416800</v>
       </c>
       <c r="B4" s="17">
-        <v>2991600</v>
+        <v>2624600</v>
       </c>
       <c r="C4" s="18">
-        <v>88476700</v>
+        <v>97114600</v>
       </c>
       <c r="D4" s="16">
         <v>295700</v>
@@ -900,13 +845,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>466200</v>
+        <v>430700</v>
       </c>
       <c r="B5" s="17">
-        <v>2820600</v>
+        <v>2567400</v>
       </c>
       <c r="C5" s="18">
-        <v>91300400</v>
+        <v>103581500</v>
       </c>
       <c r="D5" s="16">
         <v>292600</v>
@@ -953,13 +898,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>433200</v>
+        <v>425300</v>
       </c>
       <c r="B6" s="17">
-        <v>2966600</v>
+        <v>2335500</v>
       </c>
       <c r="C6" s="18">
-        <v>92750800</v>
+        <v>97340600</v>
       </c>
       <c r="D6" s="16">
         <v>297500</v>
@@ -1006,13 +951,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <v>439400</v>
+        <v>426100</v>
       </c>
       <c r="B7" s="17">
-        <v>2669000</v>
+        <v>1283000</v>
       </c>
       <c r="C7" s="18">
-        <v>91107400</v>
+        <v>97810200</v>
       </c>
       <c r="D7" s="16">
         <v>315700</v>
@@ -1038,13 +983,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>428500</v>
+        <v>441800</v>
       </c>
       <c r="B8" s="17">
-        <v>2945800</v>
+        <v>2610700</v>
       </c>
       <c r="C8" s="18">
-        <v>91911300</v>
+        <v>97651700</v>
       </c>
       <c r="D8" s="16">
         <v>306900</v>
@@ -1070,13 +1015,13 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>428300</v>
+        <v>436200</v>
       </c>
       <c r="B9" s="17">
-        <v>3059000</v>
+        <v>3011200</v>
       </c>
       <c r="C9" s="18">
-        <v>90195500</v>
+        <v>96797100</v>
       </c>
       <c r="D9" s="16">
         <v>295400</v>
@@ -1102,13 +1047,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>434700</v>
+        <v>428200</v>
       </c>
       <c r="B10" s="17">
-        <v>2931100</v>
+        <v>2497800</v>
       </c>
       <c r="C10" s="18">
-        <v>92949900</v>
+        <v>95751700</v>
       </c>
       <c r="D10" s="16">
         <v>286900</v>
@@ -1134,13 +1079,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
-        <v>467700</v>
+        <v>434000</v>
       </c>
       <c r="B11" s="17">
-        <v>2541600</v>
+        <v>2635200</v>
       </c>
       <c r="C11" s="18">
-        <v>95012000</v>
+        <v>102696400</v>
       </c>
       <c r="D11" s="16">
         <v>288900</v>
@@ -1166,13 +1111,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <v>428900</v>
+        <v>425100</v>
       </c>
       <c r="B12" s="17">
-        <v>2902900</v>
+        <v>2570600</v>
       </c>
       <c r="C12" s="18">
-        <v>96732800</v>
+        <v>91933500</v>
       </c>
       <c r="D12" s="16">
         <v>294100</v>
@@ -1198,13 +1143,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
-        <v>457300</v>
+        <v>431700</v>
       </c>
       <c r="B13" s="17">
-        <v>2225900</v>
+        <v>2581000</v>
       </c>
       <c r="C13" s="18">
-        <v>94350200</v>
+        <v>96972400</v>
       </c>
       <c r="D13" s="16">
         <v>295400</v>
@@ -1230,13 +1175,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
-        <v>446700</v>
+        <v>466800</v>
       </c>
       <c r="B14" s="17">
-        <v>2127500</v>
+        <v>2679400</v>
       </c>
       <c r="C14" s="18">
-        <v>100767800</v>
+        <v>98088100</v>
       </c>
       <c r="D14" s="16">
         <v>295400</v>
@@ -1262,13 +1207,13 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
-        <v>695400</v>
+        <v>437400</v>
       </c>
       <c r="B15" s="17">
-        <v>2859500</v>
+        <v>2373900</v>
       </c>
       <c r="C15" s="18">
-        <v>91592200</v>
+        <v>96417100</v>
       </c>
       <c r="D15" s="16">
         <v>306500</v>
@@ -1294,13 +1239,13 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
-        <v>423700</v>
+        <v>424800</v>
       </c>
       <c r="B16" s="17">
-        <v>2091100</v>
+        <v>2767600</v>
       </c>
       <c r="C16" s="18">
-        <v>89639800</v>
+        <v>97874400</v>
       </c>
       <c r="D16" s="16">
         <v>293600</v>
@@ -1326,13 +1271,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
-        <v>429800</v>
+        <v>494200</v>
       </c>
       <c r="B17" s="17">
-        <v>2668700</v>
+        <v>2813800</v>
       </c>
       <c r="C17" s="18">
-        <v>88332000</v>
+        <v>100189100</v>
       </c>
       <c r="D17" s="16">
         <v>314900</v>
@@ -1358,13 +1303,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
-        <v>429800</v>
+        <v>479200</v>
       </c>
       <c r="B18" s="17">
-        <v>2803600</v>
+        <v>2602200</v>
       </c>
       <c r="C18" s="18">
-        <v>90424100</v>
+        <v>97561000</v>
       </c>
       <c r="D18" s="16">
         <v>391800</v>
@@ -1390,13 +1335,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
-        <v>450000</v>
+        <v>452600</v>
       </c>
       <c r="B19" s="17">
-        <v>3229000</v>
+        <v>2495200</v>
       </c>
       <c r="C19" s="18">
-        <v>91049900</v>
+        <v>92841000</v>
       </c>
       <c r="D19" s="16">
         <v>336300</v>
@@ -1422,13 +1367,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
-        <v>436200</v>
+        <v>425700</v>
       </c>
       <c r="B20" s="17">
-        <v>3121000</v>
+        <v>2475400</v>
       </c>
       <c r="C20" s="18">
-        <v>90326000</v>
+        <v>97707800</v>
       </c>
       <c r="D20" s="16">
         <v>363200</v>
@@ -1454,13 +1399,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
-        <v>423900</v>
+        <v>426800</v>
       </c>
       <c r="B21" s="17">
-        <v>2986600</v>
+        <v>2662100</v>
       </c>
       <c r="C21" s="18">
-        <v>90813600</v>
+        <v>94722500</v>
       </c>
       <c r="D21" s="16">
         <v>296400</v>
@@ -1486,13 +1431,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
-        <v>425100</v>
+        <v>422900</v>
       </c>
       <c r="B22" s="17">
-        <v>2953100</v>
+        <v>3304000</v>
       </c>
       <c r="C22" s="18">
-        <v>95930400</v>
+        <v>96134900</v>
       </c>
       <c r="D22" s="16">
         <v>314700</v>
@@ -1518,13 +1463,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
-        <v>464200</v>
+        <v>471700</v>
       </c>
       <c r="B23" s="17">
-        <v>2629700</v>
+        <v>3150900</v>
       </c>
       <c r="C23" s="18">
-        <v>96606900</v>
+        <v>99885200</v>
       </c>
       <c r="D23" s="16">
         <v>291900</v>
@@ -1550,13 +1495,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
-        <v>425700</v>
+        <v>429200</v>
       </c>
       <c r="B24" s="17">
-        <v>3188900</v>
+        <v>2652600</v>
       </c>
       <c r="C24" s="18">
-        <v>101392200</v>
+        <v>97727900</v>
       </c>
       <c r="D24" s="16">
         <v>292000</v>
@@ -1582,13 +1527,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
-        <v>420800</v>
+        <v>462400</v>
       </c>
       <c r="B25" s="17">
-        <v>2255500</v>
+        <v>3202000</v>
       </c>
       <c r="C25" s="18">
-        <v>97534500</v>
+        <v>95543500</v>
       </c>
       <c r="D25" s="16">
         <v>307700</v>
@@ -1614,13 +1559,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
-        <v>428700</v>
+        <v>476900</v>
       </c>
       <c r="B26" s="17">
-        <v>2572000</v>
+        <v>3573600</v>
       </c>
       <c r="C26" s="18">
-        <v>94516400</v>
+        <v>116127600</v>
       </c>
       <c r="D26" s="16">
         <v>297200</v>
@@ -1646,13 +1591,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
-        <v>430200</v>
+        <v>461000</v>
       </c>
       <c r="B27" s="17">
-        <v>2196700</v>
+        <v>3547000</v>
       </c>
       <c r="C27" s="18">
-        <v>90650700</v>
+        <v>111718300</v>
       </c>
       <c r="D27" s="16">
         <v>294000</v>
@@ -1678,13 +1623,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>436200</v>
+        <v>427200</v>
       </c>
       <c r="B28" s="17">
-        <v>2312500</v>
+        <v>3107000</v>
       </c>
       <c r="C28" s="18">
-        <v>93157600</v>
+        <v>111264300</v>
       </c>
       <c r="D28" s="16">
         <v>297400</v>
@@ -1710,13 +1655,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>421900</v>
+        <v>441700</v>
       </c>
       <c r="B29" s="17">
-        <v>2849100</v>
+        <v>2654900</v>
       </c>
       <c r="C29" s="18">
-        <v>94866500</v>
+        <v>105515800</v>
       </c>
       <c r="D29" s="16">
         <v>308700</v>
@@ -1742,13 +1687,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>462400</v>
+        <v>459700</v>
       </c>
       <c r="B30" s="17">
-        <v>2261000</v>
+        <v>2249700</v>
       </c>
       <c r="C30" s="18">
-        <v>95115600</v>
+        <v>109052900</v>
       </c>
       <c r="D30" s="16">
         <v>305800</v>
@@ -1774,13 +1719,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>612100</v>
+        <v>430800</v>
       </c>
       <c r="B31" s="17">
-        <v>3048500</v>
+        <v>3045600</v>
       </c>
       <c r="C31" s="18">
-        <v>91913900</v>
+        <v>103664100</v>
       </c>
       <c r="D31" s="16">
         <v>306900</v>
@@ -1806,13 +1751,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>424500</v>
+        <v>425500</v>
       </c>
       <c r="B32" s="17">
-        <v>3208300</v>
+        <v>1894700</v>
       </c>
       <c r="C32" s="18">
-        <v>96563500</v>
+        <v>108861900</v>
       </c>
       <c r="D32" s="16">
         <v>294000</v>
@@ -1838,13 +1783,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
-        <v>425500</v>
+        <v>491700</v>
       </c>
       <c r="B33" s="17">
-        <v>3095900</v>
+        <v>2099800</v>
       </c>
       <c r="C33" s="18">
-        <v>93595200</v>
+        <v>94699100</v>
       </c>
       <c r="D33" s="16">
         <v>292800</v>
@@ -1870,13 +1815,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
-        <v>430800</v>
+        <v>438300</v>
       </c>
       <c r="B34" s="17">
-        <v>2887600</v>
+        <v>3192600</v>
       </c>
       <c r="C34" s="18">
-        <v>86719900</v>
+        <v>96329000</v>
       </c>
       <c r="D34" s="16">
         <v>295700</v>
@@ -1902,13 +1847,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
-        <v>426100</v>
+        <v>465400</v>
       </c>
       <c r="B35" s="17">
-        <v>2692900</v>
+        <v>3716000</v>
       </c>
       <c r="C35" s="18">
-        <v>90439400</v>
+        <v>94549300</v>
       </c>
       <c r="D35" s="16">
         <v>299300</v>
@@ -1934,13 +1879,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
-        <v>441100</v>
+        <v>437500</v>
       </c>
       <c r="B36" s="17">
-        <v>2744900</v>
+        <v>3341500</v>
       </c>
       <c r="C36" s="18">
-        <v>93679100</v>
+        <v>95458300</v>
       </c>
       <c r="D36" s="16">
         <v>301000</v>
@@ -1966,13 +1911,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
-        <v>436000</v>
+        <v>424600</v>
       </c>
       <c r="B37" s="17">
-        <v>3126900</v>
+        <v>3369300</v>
       </c>
       <c r="C37" s="18">
-        <v>89636000</v>
+        <v>96602000</v>
       </c>
       <c r="D37" s="16">
         <v>292000</v>
@@ -1998,13 +1943,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
-        <v>444900</v>
+        <v>434700</v>
       </c>
       <c r="B38" s="17">
-        <v>2785200</v>
+        <v>3894600</v>
       </c>
       <c r="C38" s="18">
-        <v>90371000</v>
+        <v>94008200</v>
       </c>
       <c r="D38" s="16">
         <v>297700</v>
@@ -2030,13 +1975,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
-        <v>428000</v>
+        <v>446700</v>
       </c>
       <c r="B39" s="17">
-        <v>2986800</v>
+        <v>2621300</v>
       </c>
       <c r="C39" s="18">
-        <v>89569100</v>
+        <v>98019600</v>
       </c>
       <c r="D39" s="16">
         <v>304700</v>
@@ -2062,13 +2007,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
-        <v>749100</v>
+        <v>425200</v>
       </c>
       <c r="B40" s="17">
-        <v>2839600</v>
+        <v>3897500</v>
       </c>
       <c r="C40" s="18">
-        <v>90537700</v>
+        <v>97055700</v>
       </c>
       <c r="D40" s="16">
         <v>302200</v>
@@ -2094,13 +2039,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
-        <v>434600</v>
+        <v>437800</v>
       </c>
       <c r="B41" s="17">
-        <v>2674600</v>
+        <v>2763300</v>
       </c>
       <c r="C41" s="18">
-        <v>90119100</v>
+        <v>97523600</v>
       </c>
       <c r="D41" s="16">
         <v>298500</v>
@@ -2126,13 +2071,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
-        <v>425000</v>
+        <v>426400</v>
       </c>
       <c r="B42" s="17">
-        <v>2868500</v>
+        <v>3668100</v>
       </c>
       <c r="C42" s="18">
-        <v>91064300</v>
+        <v>95753200</v>
       </c>
       <c r="D42" s="16">
         <v>298700</v>
@@ -2158,13 +2103,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
-        <v>427700</v>
+        <v>434200</v>
       </c>
       <c r="B43" s="17">
-        <v>2447000</v>
+        <v>3228700</v>
       </c>
       <c r="C43" s="18">
-        <v>89082100</v>
+        <v>95605000</v>
       </c>
       <c r="D43" s="16">
         <v>293800</v>
@@ -2190,13 +2135,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
-        <v>470600</v>
+        <v>424400</v>
       </c>
       <c r="B44" s="17">
-        <v>2372700</v>
+        <v>3165800</v>
       </c>
       <c r="C44" s="18">
-        <v>89242200</v>
+        <v>97119000</v>
       </c>
       <c r="D44" s="16">
         <v>294600</v>
@@ -2222,13 +2167,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
-        <v>429500</v>
+        <v>454300</v>
       </c>
       <c r="B45" s="17">
-        <v>2712500</v>
+        <v>3172200</v>
       </c>
       <c r="C45" s="18">
-        <v>88353800</v>
+        <v>95677400</v>
       </c>
       <c r="D45" s="16">
         <v>286100</v>
@@ -2254,13 +2199,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
-        <v>765300</v>
+        <v>421800</v>
       </c>
       <c r="B46" s="17">
-        <v>2846000</v>
+        <v>3005500</v>
       </c>
       <c r="C46" s="18">
-        <v>89999900</v>
+        <v>96064700</v>
       </c>
       <c r="D46" s="16">
         <v>306700</v>
@@ -2286,13 +2231,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
-        <v>430700</v>
+        <v>457900</v>
       </c>
       <c r="B47" s="17">
-        <v>2988800</v>
+        <v>3192100</v>
       </c>
       <c r="C47" s="18">
-        <v>90728000</v>
+        <v>95321700</v>
       </c>
       <c r="D47" s="16">
         <v>369900</v>
@@ -2318,13 +2263,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
-        <v>424100</v>
+        <v>436500</v>
       </c>
       <c r="B48" s="17">
-        <v>2673200</v>
+        <v>1135500</v>
       </c>
       <c r="C48" s="18">
-        <v>92312400</v>
+        <v>95927900</v>
       </c>
       <c r="D48" s="16">
         <v>291600</v>
@@ -2350,13 +2295,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
-        <v>460800</v>
+        <v>471100</v>
       </c>
       <c r="B49" s="17">
-        <v>2157200</v>
+        <v>2729600</v>
       </c>
       <c r="C49" s="18">
-        <v>91424700</v>
+        <v>94852100</v>
       </c>
       <c r="D49" s="16">
         <v>296800</v>
@@ -2382,13 +2327,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
-        <v>475300</v>
+        <v>422400</v>
       </c>
       <c r="B50" s="17">
-        <v>3018200</v>
+        <v>2579400</v>
       </c>
       <c r="C50" s="18">
-        <v>92012400</v>
+        <v>98130600</v>
       </c>
       <c r="D50" s="16">
         <v>346600</v>
@@ -2414,13 +2359,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
-        <v>765300</v>
+        <v>429500</v>
       </c>
       <c r="B51" s="17">
-        <v>3170000</v>
+        <v>2747900</v>
       </c>
       <c r="C51" s="18">
-        <v>89737100</v>
+        <v>97586100</v>
       </c>
       <c r="D51" s="16">
         <v>293700</v>
@@ -2446,13 +2391,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
-        <v>446900</v>
+        <v>435100</v>
       </c>
       <c r="B52" s="17">
-        <v>2906800</v>
+        <v>3201700</v>
       </c>
       <c r="C52" s="18">
-        <v>87713300</v>
+        <v>94633600</v>
       </c>
       <c r="D52" s="16">
         <v>298600</v>
@@ -2478,13 +2423,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
-        <v>485500</v>
+        <v>425400</v>
       </c>
       <c r="B53" s="17">
-        <v>2687800</v>
+        <v>3163600</v>
       </c>
       <c r="C53" s="18">
-        <v>85220100</v>
+        <v>103065200</v>
       </c>
       <c r="D53" s="16">
         <v>288000</v>
@@ -2510,13 +2455,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
-        <v>470500</v>
+        <v>430000</v>
       </c>
       <c r="B54" s="17">
-        <v>3092200</v>
+        <v>2598800</v>
       </c>
       <c r="C54" s="18">
-        <v>89896500</v>
+        <v>93684100</v>
       </c>
       <c r="D54" s="16">
         <v>372600</v>
@@ -2542,13 +2487,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
-        <v>440000</v>
+        <v>445300</v>
       </c>
       <c r="B55" s="17">
-        <v>2965600</v>
+        <v>2606900</v>
       </c>
       <c r="C55" s="18">
-        <v>87848100</v>
+        <v>93628200</v>
       </c>
       <c r="D55" s="16">
         <v>290300</v>
@@ -2574,13 +2519,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
-        <v>487400</v>
+        <v>432500</v>
       </c>
       <c r="B56" s="17">
-        <v>2676500</v>
+        <v>3252600</v>
       </c>
       <c r="C56" s="18">
-        <v>94666400</v>
+        <v>96961400</v>
       </c>
       <c r="D56" s="16">
         <v>297000</v>
@@ -2606,13 +2551,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
-        <v>488300</v>
+        <v>444700</v>
       </c>
       <c r="B57" s="17">
-        <v>2955500</v>
+        <v>2681100</v>
       </c>
       <c r="C57" s="18">
-        <v>89605600</v>
+        <v>99121900</v>
       </c>
       <c r="D57" s="16">
         <v>287300</v>
@@ -2638,13 +2583,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
-        <v>805200</v>
+        <v>485500</v>
       </c>
       <c r="B58" s="17">
-        <v>2870500</v>
+        <v>2549900</v>
       </c>
       <c r="C58" s="18">
-        <v>91341800</v>
+        <v>98802600</v>
       </c>
       <c r="D58" s="16">
         <v>296600</v>
@@ -2670,13 +2615,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
-        <v>443000</v>
+        <v>426600</v>
       </c>
       <c r="B59" s="17">
-        <v>2953500</v>
+        <v>3831600</v>
       </c>
       <c r="C59" s="18">
-        <v>88811100</v>
+        <v>99501400</v>
       </c>
       <c r="D59" s="16">
         <v>293600</v>
@@ -2702,13 +2647,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
-        <v>450700</v>
+        <v>425800</v>
       </c>
       <c r="B60" s="17">
-        <v>2932900</v>
+        <v>2443600</v>
       </c>
       <c r="C60" s="18">
-        <v>89320600</v>
+        <v>96898700</v>
       </c>
       <c r="D60" s="16">
         <v>295800</v>
@@ -2734,13 +2679,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
-        <v>449200</v>
+        <v>430900</v>
       </c>
       <c r="B61" s="17">
-        <v>2847500</v>
+        <v>2662400</v>
       </c>
       <c r="C61" s="18">
-        <v>89345200</v>
+        <v>96364400</v>
       </c>
       <c r="D61" s="16">
         <v>297100</v>
@@ -2766,13 +2711,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
-        <v>426900</v>
+        <v>438700</v>
       </c>
       <c r="B62" s="17">
-        <v>2399800</v>
+        <v>2984300</v>
       </c>
       <c r="C62" s="18">
-        <v>90367600</v>
+        <v>96729000</v>
       </c>
       <c r="D62" s="16">
         <v>305400</v>
@@ -2798,13 +2743,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
-        <v>432100</v>
+        <v>431100</v>
       </c>
       <c r="B63" s="17">
-        <v>3081600</v>
+        <v>2565200</v>
       </c>
       <c r="C63" s="18">
-        <v>90028700</v>
+        <v>98427500</v>
       </c>
       <c r="D63" s="16">
         <v>311900</v>
@@ -2830,13 +2775,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
-        <v>475100</v>
+        <v>427900</v>
       </c>
       <c r="B64" s="17">
-        <v>2737600</v>
+        <v>3103500</v>
       </c>
       <c r="C64" s="18">
-        <v>92471800</v>
+        <v>97268900</v>
       </c>
       <c r="D64" s="16">
         <v>294600</v>
@@ -2862,13 +2807,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
-        <v>427100</v>
+        <v>440700</v>
       </c>
       <c r="B65" s="17">
-        <v>2777000</v>
+        <v>3985900</v>
       </c>
       <c r="C65" s="18">
-        <v>87671600</v>
+        <v>100416300</v>
       </c>
       <c r="D65" s="16">
         <v>296600</v>
@@ -2894,13 +2839,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
-        <v>423100</v>
+        <v>418500</v>
       </c>
       <c r="B66" s="17">
-        <v>2875400</v>
+        <v>3259200</v>
       </c>
       <c r="C66" s="18">
-        <v>90949200</v>
+        <v>96707300</v>
       </c>
       <c r="D66" s="16">
         <v>298200</v>
@@ -2926,13 +2871,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
-        <v>425500</v>
+        <v>429200</v>
       </c>
       <c r="B67" s="17">
-        <v>2685800</v>
+        <v>3862000</v>
       </c>
       <c r="C67" s="18">
-        <v>90351300</v>
+        <v>96195000</v>
       </c>
       <c r="D67" s="16">
         <v>295000</v>
@@ -2958,13 +2903,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
-        <v>440100</v>
+        <v>443100</v>
       </c>
       <c r="B68" s="17">
-        <v>2493000</v>
+        <v>3467400</v>
       </c>
       <c r="C68" s="18">
-        <v>93550400</v>
+        <v>99390300</v>
       </c>
       <c r="D68" s="16">
         <v>297800</v>
@@ -2990,13 +2935,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
-        <v>436800</v>
+        <v>452900</v>
       </c>
       <c r="B69" s="17">
-        <v>2590700</v>
+        <v>3374700</v>
       </c>
       <c r="C69" s="18">
-        <v>89790000</v>
+        <v>96649400</v>
       </c>
       <c r="D69" s="16">
         <v>299700</v>
@@ -3022,13 +2967,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
-        <v>447000</v>
+        <v>470400</v>
       </c>
       <c r="B70" s="17">
-        <v>2587600</v>
+        <v>3878400</v>
       </c>
       <c r="C70" s="18">
-        <v>88567000</v>
+        <v>97733400</v>
       </c>
       <c r="D70" s="16">
         <v>296400</v>
@@ -3054,13 +2999,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
-        <v>429100</v>
+        <v>455400</v>
       </c>
       <c r="B71" s="17">
-        <v>2815500</v>
+        <v>1851100</v>
       </c>
       <c r="C71" s="18">
-        <v>90965900</v>
+        <v>99037300</v>
       </c>
       <c r="D71" s="16">
         <v>298000</v>
@@ -3086,13 +3031,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
-        <v>420100</v>
+        <v>464000</v>
       </c>
       <c r="B72" s="17">
-        <v>2632800</v>
+        <v>3751400</v>
       </c>
       <c r="C72" s="18">
-        <v>90211700</v>
+        <v>95616800</v>
       </c>
       <c r="D72" s="16">
         <v>284200</v>
@@ -3118,13 +3063,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
-        <v>424000</v>
+        <v>425300</v>
       </c>
       <c r="B73" s="17">
-        <v>2794000</v>
+        <v>2151600</v>
       </c>
       <c r="C73" s="18">
-        <v>89911600</v>
+        <v>94923300</v>
       </c>
       <c r="D73" s="16">
         <v>533800</v>
@@ -3150,13 +3095,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
-        <v>430600</v>
+        <v>428200</v>
       </c>
       <c r="B74" s="17">
-        <v>3026100</v>
+        <v>2468100</v>
       </c>
       <c r="C74" s="18">
-        <v>93253500</v>
+        <v>97562900</v>
       </c>
       <c r="D74" s="16">
         <v>299100</v>
@@ -3182,13 +3127,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
-        <v>430500</v>
+        <v>423600</v>
       </c>
       <c r="B75" s="17">
-        <v>2555900</v>
+        <v>2624600</v>
       </c>
       <c r="C75" s="18">
-        <v>89163300</v>
+        <v>96981800</v>
       </c>
       <c r="D75" s="16">
         <v>308000</v>
@@ -3214,13 +3159,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
-        <v>438300</v>
+        <v>427500</v>
       </c>
       <c r="B76" s="17">
-        <v>2811700</v>
+        <v>2684500</v>
       </c>
       <c r="C76" s="18">
-        <v>90213600</v>
+        <v>96912100</v>
       </c>
       <c r="D76" s="16">
         <v>310300</v>
@@ -3246,13 +3191,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
-        <v>688700</v>
+        <v>426700</v>
       </c>
       <c r="B77" s="17">
-        <v>2964700</v>
+        <v>1185700</v>
       </c>
       <c r="C77" s="18">
-        <v>89237500</v>
+        <v>98931100</v>
       </c>
       <c r="D77" s="16">
         <v>308300</v>
@@ -3278,13 +3223,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
-        <v>424000</v>
+        <v>420200</v>
       </c>
       <c r="B78" s="17">
-        <v>3029300</v>
+        <v>2697300</v>
       </c>
       <c r="C78" s="18">
-        <v>89686900</v>
+        <v>96518600</v>
       </c>
       <c r="D78" s="16">
         <v>288300</v>
@@ -3310,13 +3255,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="16">
-        <v>432200</v>
+        <v>423900</v>
       </c>
       <c r="B79" s="17">
-        <v>2883900</v>
+        <v>2668700</v>
       </c>
       <c r="C79" s="18">
-        <v>88430100</v>
+        <v>97267200</v>
       </c>
       <c r="D79" s="16">
         <v>317200</v>
@@ -3342,13 +3287,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
-        <v>423300</v>
+        <v>491100</v>
       </c>
       <c r="B80" s="17">
-        <v>2883500</v>
+        <v>2551200</v>
       </c>
       <c r="C80" s="18">
-        <v>94017600</v>
+        <v>97868500</v>
       </c>
       <c r="D80" s="16">
         <v>288100</v>
@@ -3374,13 +3319,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
-        <v>430300</v>
+        <v>458900</v>
       </c>
       <c r="B81" s="17">
-        <v>2913600</v>
+        <v>2588400</v>
       </c>
       <c r="C81" s="18">
-        <v>102945400</v>
+        <v>97528000</v>
       </c>
       <c r="D81" s="16">
         <v>296500</v>
@@ -3406,13 +3351,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="16">
-        <v>483800</v>
+        <v>423500</v>
       </c>
       <c r="B82" s="17">
-        <v>2476400</v>
+        <v>2722000</v>
       </c>
       <c r="C82" s="18">
-        <v>89947200</v>
+        <v>98037900</v>
       </c>
       <c r="D82" s="16">
         <v>296300</v>
@@ -3438,13 +3383,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
-        <v>436000</v>
+        <v>436700</v>
       </c>
       <c r="B83" s="17">
-        <v>3101300</v>
+        <v>2439400</v>
       </c>
       <c r="C83" s="18">
-        <v>90399200</v>
+        <v>94171600</v>
       </c>
       <c r="D83" s="16">
         <v>302100</v>
@@ -3470,13 +3415,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
-        <v>613200</v>
+        <v>431500</v>
       </c>
       <c r="B84" s="17">
-        <v>2148800</v>
+        <v>2796300</v>
       </c>
       <c r="C84" s="18">
-        <v>90741000</v>
+        <v>95303800</v>
       </c>
       <c r="D84" s="16">
         <v>297400</v>
@@ -3502,13 +3447,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
-        <v>422600</v>
+        <v>450900</v>
       </c>
       <c r="B85" s="17">
-        <v>3020600</v>
+        <v>2737900</v>
       </c>
       <c r="C85" s="18">
-        <v>87962000</v>
+        <v>95934800</v>
       </c>
       <c r="D85" s="16">
         <v>333900</v>
@@ -3534,13 +3479,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
-        <v>439300</v>
+        <v>444400</v>
       </c>
       <c r="B86" s="17">
-        <v>2867700</v>
+        <v>2637000</v>
       </c>
       <c r="C86" s="18">
-        <v>90603500</v>
+        <v>98119800</v>
       </c>
       <c r="D86" s="16">
         <v>300900</v>
@@ -3566,13 +3511,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
-        <v>474800</v>
+        <v>511500</v>
       </c>
       <c r="B87" s="17">
-        <v>2933500</v>
+        <v>2460000</v>
       </c>
       <c r="C87" s="18">
-        <v>92661300</v>
+        <v>98550900</v>
       </c>
       <c r="D87" s="16">
         <v>376100</v>
@@ -3598,13 +3543,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
-        <v>463700</v>
+        <v>422800</v>
       </c>
       <c r="B88" s="17">
-        <v>2892100</v>
+        <v>2688100</v>
       </c>
       <c r="C88" s="18">
-        <v>89650600</v>
+        <v>97104000</v>
       </c>
       <c r="D88" s="16">
         <v>293400</v>
@@ -3630,13 +3575,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
-        <v>430500</v>
+        <v>479900</v>
       </c>
       <c r="B89" s="17">
-        <v>2884400</v>
+        <v>2547200</v>
       </c>
       <c r="C89" s="18">
-        <v>91041700</v>
+        <v>95444900</v>
       </c>
       <c r="D89" s="16">
         <v>294400</v>
@@ -3662,13 +3607,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
-        <v>483600</v>
+        <v>433000</v>
       </c>
       <c r="B90" s="17">
-        <v>1960500</v>
+        <v>2848800</v>
       </c>
       <c r="C90" s="18">
-        <v>92663200</v>
+        <v>95296400</v>
       </c>
       <c r="D90" s="16">
         <v>296800</v>
@@ -3694,13 +3639,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="16">
-        <v>476300</v>
+        <v>431800</v>
       </c>
       <c r="B91" s="17">
-        <v>3065400</v>
+        <v>2801400</v>
       </c>
       <c r="C91" s="18">
-        <v>88822600</v>
+        <v>96949600</v>
       </c>
       <c r="D91" s="16">
         <v>318300</v>
@@ -3726,13 +3671,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="16">
-        <v>448300</v>
+        <v>481500</v>
       </c>
       <c r="B92" s="17">
-        <v>2998600</v>
+        <v>2486900</v>
       </c>
       <c r="C92" s="18">
-        <v>91839500</v>
+        <v>99558000</v>
       </c>
       <c r="D92" s="16">
         <v>316100</v>
@@ -3758,13 +3703,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
-        <v>423600</v>
+        <v>425100</v>
       </c>
       <c r="B93" s="17">
-        <v>2643200</v>
+        <v>2758400</v>
       </c>
       <c r="C93" s="18">
-        <v>90986900</v>
+        <v>97562000</v>
       </c>
       <c r="D93" s="16">
         <v>529800</v>
@@ -3790,13 +3735,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="16">
-        <v>432500</v>
+        <v>435500</v>
       </c>
       <c r="B94" s="17">
-        <v>2898400</v>
+        <v>2536700</v>
       </c>
       <c r="C94" s="18">
-        <v>89825100</v>
+        <v>99881100</v>
       </c>
       <c r="D94" s="16">
         <v>356800</v>
@@ -3822,13 +3767,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="16">
-        <v>431900</v>
+        <v>450900</v>
       </c>
       <c r="B95" s="17">
-        <v>2792100</v>
+        <v>2655600</v>
       </c>
       <c r="C95" s="18">
-        <v>91053000</v>
+        <v>96811900</v>
       </c>
       <c r="D95" s="16">
         <v>302900</v>
@@ -3854,13 +3799,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
-        <v>428600</v>
+        <v>423100</v>
       </c>
       <c r="B96" s="17">
-        <v>3059200</v>
+        <v>2601200</v>
       </c>
       <c r="C96" s="18">
-        <v>89761300</v>
+        <v>99606500</v>
       </c>
       <c r="D96" s="16">
         <v>303700</v>
@@ -3886,13 +3831,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
-        <v>420200</v>
+        <v>444800</v>
       </c>
       <c r="B97" s="17">
-        <v>2568600</v>
+        <v>2610000</v>
       </c>
       <c r="C97" s="18">
-        <v>93611800</v>
+        <v>97379300</v>
       </c>
       <c r="D97" s="16">
         <v>298000</v>
@@ -3918,13 +3863,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="16">
-        <v>437000</v>
+        <v>486900</v>
       </c>
       <c r="B98" s="17">
-        <v>3113100</v>
+        <v>2446200</v>
       </c>
       <c r="C98" s="18">
-        <v>88998600</v>
+        <v>97778500</v>
       </c>
       <c r="D98" s="16">
         <v>296300</v>
@@ -3950,13 +3895,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
-        <v>472600</v>
+        <v>440800</v>
       </c>
       <c r="B99" s="17">
-        <v>2869200</v>
+        <v>2677000</v>
       </c>
       <c r="C99" s="18">
-        <v>91458600</v>
+        <v>95426900</v>
       </c>
       <c r="D99" s="16">
         <v>297700</v>
@@ -3982,13 +3927,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="16">
-        <v>434100</v>
+        <v>430000</v>
       </c>
       <c r="B100" s="17">
-        <v>2987700</v>
+        <v>2716900</v>
       </c>
       <c r="C100" s="18">
-        <v>88851200</v>
+        <v>98360900</v>
       </c>
       <c r="D100" s="16">
         <v>321200</v>
@@ -4014,13 +3959,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="16">
-        <v>438900</v>
+        <v>458000</v>
       </c>
       <c r="B101" s="17">
-        <v>3089500</v>
+        <v>2428100</v>
       </c>
       <c r="C101" s="18">
-        <v>92408500</v>
+        <v>94990600</v>
       </c>
       <c r="D101" s="16">
         <v>298700</v>
@@ -4046,13 +3991,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="19">
-        <v>426400</v>
+        <v>472100</v>
       </c>
       <c r="B102" s="20">
-        <v>3060900</v>
+        <v>2727600</v>
       </c>
       <c r="C102" s="21">
-        <v>87969200</v>
+        <v>96581500</v>
       </c>
       <c r="D102" s="19">
         <v>390900</v>
@@ -4085,6 +4030,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Laptop Data Graphs
</commit_message>
<xml_diff>
--- a/Results Summary Laptop.xlsx
+++ b/Results Summary Laptop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\Projects\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB34DBE0-332C-4D8C-9C15-09A29745163C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398375B4-6450-4027-BD30-01A461A24FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,6 +353,61 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>117473</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D127505F-9106-2886-3D9C-140A2F7DB1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8594723" y="1343025"/>
+          <a:ext cx="10007602" cy="5629276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -653,7 +708,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B102"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,5 +4085,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>